<commit_message>
chore: atualizar arquivos de geração e Excel
</commit_message>
<xml_diff>
--- a/src/utils/Relatório BOs.xlsx
+++ b/src/utils/Relatório BOs.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Página1'!$A$1:$T$2</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Página1'!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -75,37 +75,37 @@
     <t>dataVehicleSituation</t>
   </si>
   <si>
-    <t>WESLEY FERNANDO LEANDRO RODRIGUES</t>
-  </si>
-  <si>
-    <t>TKL-5A56</t>
+    <t>laion de Lara silva</t>
+  </si>
+  <si>
+    <t>UDT-1E38</t>
   </si>
   <si>
     <t>Mottu Sport ESD</t>
   </si>
   <si>
-    <t>2026-01-15 05:04:33.000000 UTC</t>
-  </si>
-  <si>
-    <t>-22.326294, -49.074837</t>
+    <t>2026-01-16 04:04:57.000000 UTC</t>
+  </si>
+  <si>
+    <t>-23.975288, -48.864197</t>
   </si>
   <si>
     <t>Verificar</t>
   </si>
   <si>
-    <t>Rua João Baptista Garcia Filho, 234, Bauru - SP, 17047245</t>
-  </si>
-  <si>
-    <t>2026-01-05 04:41:16.300000 UTC</t>
-  </si>
-  <si>
-    <t>Eduardo Hungaro Martin</t>
-  </si>
-  <si>
-    <t>92EC10BGSSM053116</t>
-  </si>
-  <si>
-    <t>Mottu Bauru</t>
+    <t>R. Higino Marques, 87, Itapeva - SP, 18407120</t>
+  </si>
+  <si>
+    <t>2026-01-15 04:41:18.020000 UTC</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>92EC10BHSSM055161</t>
+  </si>
+  <si>
+    <t>Mottu Itapeva</t>
   </si>
   <si>
     <t>Apropriacao Indebita</t>
@@ -372,8 +372,7 @@
     <col customWidth="1" min="14" max="14" width="12.67"/>
     <col customWidth="1" min="15" max="15" width="24.89"/>
     <col customWidth="1" min="16" max="16" width="20.44"/>
-    <col customWidth="1" min="17" max="17" width="16.22"/>
-    <col customWidth="1" min="18" max="18" width="13.78"/>
+    <col customWidth="1" min="17" max="18" width="16.22"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -440,10 +439,10 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="B2" s="1">
-        <v>175439.0</v>
+        <v>177745.0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -476,10 +475,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="1">
-        <v>5242552.0</v>
+        <v>4750020.0</v>
       </c>
       <c r="N2" s="1">
-        <v>4876496.0</v>
+        <v>4429466.0</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>28</v>
@@ -562,30 +561,8 @@
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$A$1:$T$2"/>
+  <autoFilter ref="$A$1:$T$1"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>